<commit_message>
updated powerblade 3v2 parts spreadsheet while assembling pogos
</commit_message>
<xml_diff>
--- a/eagle/powerblade/past_rev/3v2/powerblade_3v2.xlsx
+++ b/eagle/powerblade/past_rev/3v2/powerblade_3v2.xlsx
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="237">
   <si>
     <t>Part</t>
   </si>
@@ -750,6 +750,9 @@
   </si>
   <si>
     <t>RI1 RI2</t>
+  </si>
+  <si>
+    <t>10+4</t>
   </si>
 </sst>
 </file>
@@ -785,20 +788,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <fill>
         <patternFill>
@@ -1107,10 +1106,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K62"/>
+  <dimension ref="A1:L62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="F61" sqref="F61"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1123,9 +1122,10 @@
     <col min="7" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1160,7 +1160,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>58</v>
       </c>
@@ -1189,8 +1189,11 @@
         <f>MAX(0,2*H2-G2)</f>
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L2" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>202</v>
       </c>
@@ -1222,8 +1225,11 @@
       <c r="K3" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L3" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>194</v>
       </c>
@@ -1249,8 +1255,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L4" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>211</v>
       </c>
@@ -1276,8 +1285,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L5" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>208</v>
       </c>
@@ -1303,8 +1315,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L6" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>190</v>
       </c>
@@ -1330,8 +1345,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L7" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>198</v>
       </c>
@@ -1357,8 +1375,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L8" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>112</v>
       </c>
@@ -1384,8 +1405,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L9" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>32</v>
       </c>
@@ -1414,8 +1438,11 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L10" s="1" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>63</v>
       </c>
@@ -1444,8 +1471,11 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L11" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>72</v>
       </c>
@@ -1474,8 +1504,11 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L12" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>230</v>
       </c>
@@ -1504,8 +1537,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L13" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>227</v>
       </c>
@@ -1534,8 +1570,11 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L14" s="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>55</v>
       </c>
@@ -1564,8 +1603,11 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L15" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>45</v>
       </c>
@@ -1594,8 +1636,11 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L16" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>52</v>
       </c>
@@ -1624,8 +1669,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L17" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>41</v>
       </c>
@@ -1654,8 +1702,11 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L18" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>228</v>
       </c>
@@ -1684,8 +1735,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L19" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>16</v>
       </c>
@@ -1714,8 +1768,11 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L20" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>22</v>
       </c>
@@ -1741,8 +1798,11 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L21" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>229</v>
       </c>
@@ -1771,8 +1831,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L22" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>105</v>
       </c>
@@ -1801,8 +1864,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L23" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>93</v>
       </c>
@@ -1831,8 +1897,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L24" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>66</v>
       </c>
@@ -1861,8 +1930,11 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L25" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>231</v>
       </c>
@@ -1891,8 +1963,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L26" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>69</v>
       </c>
@@ -1921,8 +1996,11 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L27" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>11</v>
       </c>
@@ -1954,8 +2032,11 @@
       <c r="K28" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L28" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>220</v>
       </c>
@@ -1981,8 +2062,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L29" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>99</v>
       </c>
@@ -2008,8 +2092,11 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L30" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>103</v>
       </c>
@@ -2035,8 +2122,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L31" s="1" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>215</v>
       </c>
@@ -2065,8 +2155,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L32" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>79</v>
       </c>
@@ -2092,8 +2185,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L33" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>75</v>
       </c>
@@ -2119,8 +2215,11 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L34" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>86</v>
       </c>
@@ -2147,7 +2246,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>35</v>
       </c>
@@ -2166,8 +2265,11 @@
       <c r="F36" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L36" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>83</v>
       </c>
@@ -2183,8 +2285,11 @@
       <c r="F37" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L37" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>90</v>
       </c>
@@ -2200,8 +2305,11 @@
       <c r="F38" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L38" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>108</v>
       </c>
@@ -2227,8 +2335,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L39" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>154</v>
       </c>
@@ -2254,8 +2365,11 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L40" s="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>232</v>
       </c>
@@ -2284,8 +2398,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L41" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>163</v>
       </c>
@@ -2314,8 +2431,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L42" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>177</v>
       </c>
@@ -2344,8 +2464,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L43" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>142</v>
       </c>
@@ -2374,8 +2497,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L44" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>168</v>
       </c>
@@ -2404,8 +2530,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L45" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>147</v>
       </c>
@@ -2434,8 +2563,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L46" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>139</v>
       </c>
@@ -2464,8 +2596,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L47" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>115</v>
       </c>
@@ -2491,8 +2626,11 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L48" s="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>174</v>
       </c>
@@ -2521,8 +2659,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L49" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>233</v>
       </c>
@@ -2551,8 +2692,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L50" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>180</v>
       </c>
@@ -2578,8 +2722,11 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L51" s="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>160</v>
       </c>
@@ -2608,8 +2755,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L52" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>136</v>
       </c>
@@ -2638,8 +2788,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L53" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>234</v>
       </c>
@@ -2668,8 +2821,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L54" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>121</v>
       </c>
@@ -2698,8 +2854,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L55" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>151</v>
       </c>
@@ -2728,8 +2887,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L56" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>171</v>
       </c>
@@ -2758,8 +2920,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L57" s="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>235</v>
       </c>
@@ -2788,8 +2953,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L58" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>126</v>
       </c>
@@ -2818,8 +2986,11 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L59" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>157</v>
       </c>
@@ -2848,8 +3019,11 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L60" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>185</v>
       </c>
@@ -2872,8 +3046,11 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L61" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>224</v>
       </c>
@@ -2901,6 +3078,9 @@
       </c>
       <c r="K62" t="s">
         <v>226</v>
+      </c>
+      <c r="L62" s="1">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -2908,7 +3088,7 @@
     <sortCondition ref="F2:F79"/>
   </sortState>
   <conditionalFormatting sqref="I2:I62">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
continued to thrash the ppowerblade 3v2 parts list for my own purposes (assembling 3v2)
</commit_message>
<xml_diff>
--- a/eagle/powerblade/past_rev/3v2/powerblade_3v2.xlsx
+++ b/eagle/powerblade/past_rev/3v2/powerblade_3v2.xlsx
@@ -797,7 +797,21 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="3">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1106,10 +1120,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L62"/>
+  <dimension ref="A1:N62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N24" sqref="N24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1125,7 +1139,7 @@
     <col min="12" max="12" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1160,7 +1174,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>58</v>
       </c>
@@ -1192,8 +1206,16 @@
       <c r="L2" s="1">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M2">
+        <f>L2-H2</f>
+        <v>9</v>
+      </c>
+      <c r="N2">
+        <f>M2-2*H2</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>202</v>
       </c>
@@ -1228,8 +1250,16 @@
       <c r="L3" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M3">
+        <f t="shared" ref="M3:M62" si="1">L3-H3</f>
+        <v>4</v>
+      </c>
+      <c r="N3">
+        <f t="shared" ref="N3:N62" si="2">M3-2*H3</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>194</v>
       </c>
@@ -1258,8 +1288,16 @@
       <c r="L4" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M4">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="N4">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>211</v>
       </c>
@@ -1288,8 +1326,16 @@
       <c r="L5" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M5">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="N5">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>208</v>
       </c>
@@ -1318,8 +1364,16 @@
       <c r="L6" s="1">
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M6">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="N6">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>190</v>
       </c>
@@ -1348,8 +1402,16 @@
       <c r="L7" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M7">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="N7">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>198</v>
       </c>
@@ -1378,8 +1440,16 @@
       <c r="L8" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M8">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="N8">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>112</v>
       </c>
@@ -1408,8 +1478,16 @@
       <c r="L9" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M9">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="N9">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>32</v>
       </c>
@@ -1441,8 +1519,16 @@
       <c r="L10" s="1" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M10" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="N10" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>63</v>
       </c>
@@ -1474,8 +1560,16 @@
       <c r="L11" s="1">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M11">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="N11">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>72</v>
       </c>
@@ -1507,8 +1601,16 @@
       <c r="L12" s="1">
         <v>10</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M12">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="N12">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>230</v>
       </c>
@@ -1540,8 +1642,16 @@
       <c r="L13" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M13">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="N13">
+        <f t="shared" si="2"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>227</v>
       </c>
@@ -1573,8 +1683,16 @@
       <c r="L14" s="1">
         <v>50</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M14">
+        <f t="shared" si="1"/>
+        <v>43</v>
+      </c>
+      <c r="N14">
+        <f t="shared" si="2"/>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>55</v>
       </c>
@@ -1606,8 +1724,16 @@
       <c r="L15" s="1">
         <v>10</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M15">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="N15">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>45</v>
       </c>
@@ -1639,8 +1765,16 @@
       <c r="L16" s="1">
         <v>10</v>
       </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M16">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="N16">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>52</v>
       </c>
@@ -1672,8 +1806,16 @@
       <c r="L17" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M17">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="N17">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>41</v>
       </c>
@@ -1705,8 +1847,16 @@
       <c r="L18" s="1">
         <v>10</v>
       </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M18">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="N18">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>228</v>
       </c>
@@ -1738,8 +1888,16 @@
       <c r="L19" s="1">
         <v>15</v>
       </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M19">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="N19">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>16</v>
       </c>
@@ -1771,8 +1929,16 @@
       <c r="L20" s="1">
         <v>10</v>
       </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M20">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="N20">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>22</v>
       </c>
@@ -1801,8 +1967,16 @@
       <c r="L21" s="1">
         <v>10</v>
       </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M21">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="N21">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>229</v>
       </c>
@@ -1832,10 +2006,18 @@
         <v>0</v>
       </c>
       <c r="L22" s="1">
+        <v>10</v>
+      </c>
+      <c r="M22">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="N22">
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>105</v>
       </c>
@@ -1867,8 +2049,16 @@
       <c r="L23" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M23">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="N23">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>93</v>
       </c>
@@ -1900,8 +2090,16 @@
       <c r="L24" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M24">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="N24">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>66</v>
       </c>
@@ -1933,8 +2131,16 @@
       <c r="L25" s="1">
         <v>10</v>
       </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M25">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="N25">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>231</v>
       </c>
@@ -1966,8 +2172,16 @@
       <c r="L26" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M26">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="N26">
+        <f t="shared" si="2"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>69</v>
       </c>
@@ -1999,8 +2213,16 @@
       <c r="L27" s="1">
         <v>10</v>
       </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M27">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="N27">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>11</v>
       </c>
@@ -2035,8 +2257,16 @@
       <c r="L28" s="1">
         <v>7</v>
       </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M28">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="N28">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>220</v>
       </c>
@@ -2065,8 +2295,16 @@
       <c r="L29" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M29">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="N29">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>99</v>
       </c>
@@ -2095,8 +2333,16 @@
       <c r="L30" s="1">
         <v>10</v>
       </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M30">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="N30">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>103</v>
       </c>
@@ -2125,8 +2371,16 @@
       <c r="L31" s="1" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M31" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="N31" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>215</v>
       </c>
@@ -2158,8 +2412,16 @@
       <c r="L32" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M32">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="N32">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>79</v>
       </c>
@@ -2188,8 +2450,16 @@
       <c r="L33" s="1">
         <v>10</v>
       </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M33">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="N33">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>75</v>
       </c>
@@ -2218,8 +2488,16 @@
       <c r="L34" s="1">
         <v>10</v>
       </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M34">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="N34">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>86</v>
       </c>
@@ -2245,8 +2523,16 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M35">
+        <f t="shared" si="1"/>
+        <v>-4</v>
+      </c>
+      <c r="N35">
+        <f t="shared" si="2"/>
+        <v>-12</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>35</v>
       </c>
@@ -2268,8 +2554,16 @@
       <c r="L36" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M36" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="N36" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>83</v>
       </c>
@@ -2288,8 +2582,16 @@
       <c r="L37" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M37" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="N37" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>90</v>
       </c>
@@ -2308,8 +2610,16 @@
       <c r="L38" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M38" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="N38" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>108</v>
       </c>
@@ -2338,8 +2648,16 @@
       <c r="L39" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M39">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="N39">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>154</v>
       </c>
@@ -2368,8 +2686,16 @@
       <c r="L40" s="1">
         <v>50</v>
       </c>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M40">
+        <f t="shared" si="1"/>
+        <v>49</v>
+      </c>
+      <c r="N40">
+        <f t="shared" si="2"/>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>232</v>
       </c>
@@ -2401,8 +2727,16 @@
       <c r="L41" s="1">
         <v>20</v>
       </c>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M41">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="N41">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>163</v>
       </c>
@@ -2434,8 +2768,16 @@
       <c r="L42" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M42">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="N42">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>177</v>
       </c>
@@ -2467,8 +2809,16 @@
       <c r="L43" s="1">
         <v>20</v>
       </c>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M43">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+      <c r="N43">
+        <f t="shared" si="2"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>142</v>
       </c>
@@ -2500,8 +2850,16 @@
       <c r="L44" s="1">
         <v>20</v>
       </c>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M44">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+      <c r="N44">
+        <f t="shared" si="2"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>168</v>
       </c>
@@ -2533,8 +2891,16 @@
       <c r="L45" s="1">
         <v>20</v>
       </c>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M45">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+      <c r="N45">
+        <f t="shared" si="2"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>147</v>
       </c>
@@ -2566,8 +2932,16 @@
       <c r="L46" s="1">
         <v>20</v>
       </c>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M46">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+      <c r="N46">
+        <f t="shared" si="2"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>139</v>
       </c>
@@ -2599,8 +2973,16 @@
       <c r="L47" s="1">
         <v>20</v>
       </c>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M47">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+      <c r="N47">
+        <f t="shared" si="2"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>115</v>
       </c>
@@ -2629,8 +3011,16 @@
       <c r="L48" s="1">
         <v>50</v>
       </c>
-    </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M48">
+        <f t="shared" si="1"/>
+        <v>49</v>
+      </c>
+      <c r="N48">
+        <f t="shared" si="2"/>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>174</v>
       </c>
@@ -2662,8 +3052,16 @@
       <c r="L49" s="1">
         <v>20</v>
       </c>
-    </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M49">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+      <c r="N49">
+        <f t="shared" si="2"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>233</v>
       </c>
@@ -2695,8 +3093,16 @@
       <c r="L50" s="1">
         <v>20</v>
       </c>
-    </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M50">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="N50">
+        <f t="shared" si="2"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>180</v>
       </c>
@@ -2725,8 +3131,16 @@
       <c r="L51" s="1">
         <v>50</v>
       </c>
-    </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M51">
+        <f t="shared" si="1"/>
+        <v>49</v>
+      </c>
+      <c r="N51">
+        <f t="shared" si="2"/>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>160</v>
       </c>
@@ -2758,8 +3172,16 @@
       <c r="L52" s="1">
         <v>20</v>
       </c>
-    </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M52">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+      <c r="N52">
+        <f t="shared" si="2"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>136</v>
       </c>
@@ -2791,8 +3213,16 @@
       <c r="L53" s="1">
         <v>20</v>
       </c>
-    </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M53">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+      <c r="N53">
+        <f t="shared" si="2"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>234</v>
       </c>
@@ -2824,8 +3254,16 @@
       <c r="L54" s="1">
         <v>20</v>
       </c>
-    </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M54">
+        <f t="shared" si="1"/>
+        <v>17</v>
+      </c>
+      <c r="N54">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>121</v>
       </c>
@@ -2857,8 +3295,16 @@
       <c r="L55" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M55">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="N55">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>151</v>
       </c>
@@ -2890,8 +3336,16 @@
       <c r="L56" s="1">
         <v>20</v>
       </c>
-    </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M56">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+      <c r="N56">
+        <f t="shared" si="2"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>171</v>
       </c>
@@ -2923,8 +3377,16 @@
       <c r="L57" s="1">
         <v>50</v>
       </c>
-    </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M57">
+        <f t="shared" si="1"/>
+        <v>49</v>
+      </c>
+      <c r="N57">
+        <f t="shared" si="2"/>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>235</v>
       </c>
@@ -2956,8 +3418,16 @@
       <c r="L58" s="1">
         <v>20</v>
       </c>
-    </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M58">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="N58">
+        <f t="shared" si="2"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>126</v>
       </c>
@@ -2989,8 +3459,16 @@
       <c r="L59" s="1">
         <v>10</v>
       </c>
-    </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M59">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="N59">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>157</v>
       </c>
@@ -3022,8 +3500,16 @@
       <c r="L60" s="1">
         <v>10</v>
       </c>
-    </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M60">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="N60">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>185</v>
       </c>
@@ -3049,8 +3535,16 @@
       <c r="L61" s="1">
         <v>10</v>
       </c>
-    </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M61">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="N61">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>224</v>
       </c>
@@ -3081,6 +3575,14 @@
       </c>
       <c r="L62" s="1">
         <v>10</v>
+      </c>
+      <c r="M62">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="N62">
+        <f t="shared" si="2"/>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -3088,7 +3590,12 @@
     <sortCondition ref="F2:F79"/>
   </sortState>
   <conditionalFormatting sqref="I2:I62">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N2:N62">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>